<commit_message>
vocmap writes a excel
</commit_message>
<xml_diff>
--- a/zml2lido/data/vocmap.xlsx
+++ b/zml2lido/data/vocmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>doc</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>application/vnd.ms-excel</t>
+  </si>
+  <si>
+    <t>scope</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,7 +437,9 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>